<commit_message>
add new menu file
</commit_message>
<xml_diff>
--- a/public/menu.xlsx
+++ b/public/menu.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/i558154/Downloads/teatar-beer-bar---digital-menu/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4B54E4A-47BB-D940-967D-BAD17B0E3E56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2CEA926-2586-E24D-809E-E23FE03F8A6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="660" windowWidth="34560" windowHeight="19840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="34560" windowHeight="19720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="110">
   <si>
     <t>Naziv</t>
   </si>
@@ -277,18 +277,9 @@
     <t>RUBINOV VINJAK</t>
   </si>
   <si>
-    <t>SANGRIA VOCNO VINO</t>
-  </si>
-  <si>
     <t>SCHWEPPES BITTER LEMON</t>
   </si>
   <si>
-    <t>SCHWEPPES MOJITO</t>
-  </si>
-  <si>
-    <t>SCHWEPPES PINK</t>
-  </si>
-  <si>
     <t>SCHWEPPES TONIC WATER</t>
   </si>
   <si>
@@ -344,9 +335,6 @@
   </si>
   <si>
     <t>VALJEVSKO TOCENO PIVO 0.5</t>
-  </si>
-  <si>
-    <t>VINO KASTEL</t>
   </si>
   <si>
     <t>VITAMINSKI</t>
@@ -724,14 +712,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E96"/>
+  <dimension ref="A1:E92"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="A99" sqref="A99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="37.6640625" customWidth="1"/>
     <col min="2" max="2" width="48.33203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1879,7 +1868,7 @@
         <v>85</v>
       </c>
       <c r="B68" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="C68" t="s">
         <v>7</v>
@@ -1888,7 +1877,7 @@
         <v>8</v>
       </c>
       <c r="E68">
-        <v>300</v>
+        <v>170</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
@@ -1913,13 +1902,13 @@
         <v>87</v>
       </c>
       <c r="B70" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C70" t="s">
         <v>7</v>
       </c>
       <c r="D70" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E70">
         <v>150</v>
@@ -1930,7 +1919,7 @@
         <v>88</v>
       </c>
       <c r="B71" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="C71" t="s">
         <v>7</v>
@@ -1939,7 +1928,7 @@
         <v>8</v>
       </c>
       <c r="E71">
-        <v>150</v>
+        <v>140</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
@@ -1947,16 +1936,16 @@
         <v>89</v>
       </c>
       <c r="B72" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="C72" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D72" t="s">
         <v>8</v>
       </c>
       <c r="E72">
-        <v>170</v>
+        <v>200</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
@@ -1970,10 +1959,10 @@
         <v>7</v>
       </c>
       <c r="D73" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E73">
-        <v>150</v>
+        <v>130</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
@@ -1981,16 +1970,16 @@
         <v>91</v>
       </c>
       <c r="B74" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C74" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D74" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E74">
-        <v>140</v>
+        <v>240</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
@@ -1998,16 +1987,16 @@
         <v>92</v>
       </c>
       <c r="B75" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="C75" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D75" t="s">
         <v>8</v>
       </c>
       <c r="E75">
-        <v>200</v>
+        <v>240</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
@@ -2024,7 +2013,7 @@
         <v>8</v>
       </c>
       <c r="E76">
-        <v>100</v>
+        <v>240</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
@@ -2032,16 +2021,16 @@
         <v>94</v>
       </c>
       <c r="B77" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="C77" t="s">
         <v>10</v>
       </c>
       <c r="D77" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E77">
-        <v>240</v>
+        <v>220</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
@@ -2049,7 +2038,7 @@
         <v>95</v>
       </c>
       <c r="B78" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="C78" t="s">
         <v>7</v>
@@ -2058,7 +2047,7 @@
         <v>8</v>
       </c>
       <c r="E78">
-        <v>240</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
@@ -2066,7 +2055,7 @@
         <v>96</v>
       </c>
       <c r="B79" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C79" t="s">
         <v>7</v>
@@ -2075,7 +2064,7 @@
         <v>8</v>
       </c>
       <c r="E79">
-        <v>240</v>
+        <v>230</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
@@ -2083,16 +2072,16 @@
         <v>97</v>
       </c>
       <c r="B80" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="C80" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D80" t="s">
         <v>8</v>
       </c>
       <c r="E80">
-        <v>220</v>
+        <v>230</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
@@ -2100,7 +2089,7 @@
         <v>98</v>
       </c>
       <c r="B81" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="C81" t="s">
         <v>7</v>
@@ -2109,7 +2098,7 @@
         <v>8</v>
       </c>
       <c r="E81">
-        <v>1100</v>
+        <v>190</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
@@ -2126,7 +2115,7 @@
         <v>8</v>
       </c>
       <c r="E82">
-        <v>230</v>
+        <v>100</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
@@ -2134,16 +2123,16 @@
         <v>100</v>
       </c>
       <c r="B83" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C83" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D83" t="s">
         <v>8</v>
       </c>
       <c r="E83">
-        <v>230</v>
+        <v>250</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
@@ -2151,7 +2140,7 @@
         <v>101</v>
       </c>
       <c r="B84" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="C84" t="s">
         <v>7</v>
@@ -2160,7 +2149,7 @@
         <v>8</v>
       </c>
       <c r="E84">
-        <v>190</v>
+        <v>350</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
@@ -2168,7 +2157,7 @@
         <v>102</v>
       </c>
       <c r="B85" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C85" t="s">
         <v>7</v>
@@ -2177,7 +2166,7 @@
         <v>8</v>
       </c>
       <c r="E85">
-        <v>100</v>
+        <v>150</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
@@ -2185,16 +2174,16 @@
         <v>103</v>
       </c>
       <c r="B86" t="s">
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="C86" t="s">
         <v>10</v>
       </c>
       <c r="D86" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E86">
-        <v>250</v>
+        <v>180</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
@@ -2202,16 +2191,16 @@
         <v>104</v>
       </c>
       <c r="B87" t="s">
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="C87" t="s">
         <v>7</v>
       </c>
       <c r="D87" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E87">
-        <v>350</v>
+        <v>230</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
@@ -2219,16 +2208,16 @@
         <v>105</v>
       </c>
       <c r="B88" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C88" t="s">
         <v>7</v>
       </c>
       <c r="D88" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E88">
-        <v>150</v>
+        <v>140</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
@@ -2236,16 +2225,16 @@
         <v>106</v>
       </c>
       <c r="B89" t="s">
-        <v>48</v>
+        <v>15</v>
       </c>
       <c r="C89" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D89" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E89">
-        <v>180</v>
+        <v>200</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
@@ -2253,16 +2242,16 @@
         <v>107</v>
       </c>
       <c r="B90" t="s">
-        <v>48</v>
+        <v>15</v>
       </c>
       <c r="C90" t="s">
         <v>7</v>
       </c>
       <c r="D90" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E90">
-        <v>230</v>
+        <v>350</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.2">
@@ -2270,7 +2259,7 @@
         <v>108</v>
       </c>
       <c r="B91" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="C91" t="s">
         <v>7</v>
@@ -2279,7 +2268,7 @@
         <v>8</v>
       </c>
       <c r="E91">
-        <v>270</v>
+        <v>250</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
@@ -2287,89 +2276,21 @@
         <v>109</v>
       </c>
       <c r="B92" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="C92" t="s">
         <v>7</v>
       </c>
       <c r="D92" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E92">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A93" t="s">
-        <v>110</v>
-      </c>
-      <c r="B93" t="s">
-        <v>15</v>
-      </c>
-      <c r="C93" t="s">
-        <v>7</v>
-      </c>
-      <c r="D93" t="s">
-        <v>8</v>
-      </c>
-      <c r="E93">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A94" t="s">
-        <v>111</v>
-      </c>
-      <c r="B94" t="s">
-        <v>15</v>
-      </c>
-      <c r="C94" t="s">
-        <v>7</v>
-      </c>
-      <c r="D94" t="s">
-        <v>8</v>
-      </c>
-      <c r="E94">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A95" t="s">
-        <v>112</v>
-      </c>
-      <c r="B95" t="s">
-        <v>15</v>
-      </c>
-      <c r="C95" t="s">
-        <v>7</v>
-      </c>
-      <c r="D95" t="s">
-        <v>8</v>
-      </c>
-      <c r="E95">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A96" t="s">
-        <v>113</v>
-      </c>
-      <c r="B96" t="s">
-        <v>34</v>
-      </c>
-      <c r="C96" t="s">
-        <v>7</v>
-      </c>
-      <c r="D96" t="s">
-        <v>8</v>
-      </c>
-      <c r="E96">
         <v>400</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Nevažeća grupa" error="Molimo izaberite grupu iz ponuđene liste." sqref="B2:B1000" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Nevažeća grupa" error="Molimo izaberite grupu iz ponuđene liste." sqref="B95:B1000 B2:B92" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"GAZIRANI I NEGAZIRANI SOKOVI,INDUSTRIJSKA FLASIRANA PIVA,INDUSTRIJSKA TOCENA PIVA,KAFE I ČAJEVI,KRAFT TOCENA PIVA,SEJKOVI,VINA,ZESTINE"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
promenjen naziv kategorije, dodata rec caj ispred
</commit_message>
<xml_diff>
--- a/public/menu.xlsx
+++ b/public/menu.xlsx
@@ -527,12 +527,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>ALIBABA</t>
+          <t>ČAJ ALIBABA</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>KAFE I ČAJEVI</t>
+          <t>TOPLI NAPICI</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -977,12 +977,12 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>CRVENA POMORANDZA</t>
+          <t>ČAJ CRVENA POMORANDZA</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>KAFE I ČAJEVI</t>
+          <t>TOPLI NAPICI</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1082,7 +1082,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>KAFE I ČAJEVI</t>
+          <t>TOPLI NAPICI</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1202,12 +1202,12 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>JAGODA KREM</t>
+          <t>ČAJ JAGODA KREM</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>KAFE I ČAJEVI</t>
+          <t>TOPLI NAPICI</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1407,7 +1407,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>KAFE I ČAJEVI</t>
+          <t>TOPLI NAPICI</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1427,12 +1427,12 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>KIBA FLIP</t>
+          <t>ČAJ KIBA FLIP</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>KAFE I ČAJEVI</t>
+          <t>TOPLI NAPICI</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1677,12 +1677,12 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>LEDENO DOBA</t>
+          <t>ČAJ LEDENO DOBA</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>KAFE I ČAJEVI</t>
+          <t>TOPLI NAPICI</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -1757,7 +1757,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>KAFE I ČAJEVI</t>
+          <t>TOPLI NAPICI</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -1882,7 +1882,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>KAFE I ČAJEVI</t>
+          <t>TOPLI NAPICI</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -2202,12 +2202,12 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>SMOKVA MARAKUJA</t>
+          <t>ČAJ SMOKVA MARAKUJA</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>KAFE I ČAJEVI</t>
+          <t>TOPLI NAPICI</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -2407,7 +2407,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>KAFE I ČAJEVI</t>
+          <t>TOPLI NAPICI</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -2432,7 +2432,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>KAFE I ČAJEVI</t>
+          <t>TOPLI NAPICI</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -2482,7 +2482,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>KAFE I ČAJEVI</t>
+          <t>TOPLI NAPICI</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -2632,7 +2632,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>KAFE I ČAJEVI</t>
+          <t>TOPLI NAPICI</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">

</xml_diff>